<commit_message>
working on main functions and building
</commit_message>
<xml_diff>
--- a/documentation/TN7_Test.xlsx
+++ b/documentation/TN7_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25620" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Churches" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="395">
   <si>
     <t>Church</t>
   </si>
@@ -1173,42 +1173,9 @@
     <t>Female</t>
   </si>
   <si>
-    <t>UBC</t>
-  </si>
-  <si>
-    <t>Unassigned</t>
-  </si>
-  <si>
-    <t>Sutton</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Floor 1 Rooms</t>
-  </si>
-  <si>
-    <t>Floor 1 Capacity</t>
-  </si>
-  <si>
-    <t>Floor 2 Rooms</t>
-  </si>
-  <si>
-    <t>Floor 2 Capacity</t>
-  </si>
-  <si>
-    <t>Floor 3 Rooms</t>
-  </si>
-  <si>
-    <t>Floor 3 Capacity</t>
-  </si>
-  <si>
-    <t>Floor 4 Rooms</t>
-  </si>
-  <si>
-    <t>Floor 4 Capacity</t>
-  </si>
-  <si>
     <t>Eastview</t>
   </si>
   <si>
@@ -1219,6 +1186,27 @@
   </si>
   <si>
     <t>Champaign</t>
+  </si>
+  <si>
+    <t>Number of Floors</t>
+  </si>
+  <si>
+    <t>Room Type 1 Capacity</t>
+  </si>
+  <si>
+    <t>Room Type 1 Quantity</t>
+  </si>
+  <si>
+    <t>Room Type 2 Capacity</t>
+  </si>
+  <si>
+    <t>Room Type 2 Quantity</t>
+  </si>
+  <si>
+    <t>Room Type 3 Capacity</t>
+  </si>
+  <si>
+    <t>Room Type 3 Quantity</t>
   </si>
 </sst>
 </file>
@@ -1301,8 +1289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1336,15 +1330,21 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1676,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1758,13 +1758,13 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="D2" s="2">
         <v>61704</v>
@@ -1800,13 +1800,13 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="D3" s="2">
         <v>61820</v>
@@ -2982,10 +2982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2998,39 +2998,36 @@
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>378</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="J1" s="7" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>379</v>
       </c>
@@ -3038,118 +3035,110 @@
         <v>380</v>
       </c>
       <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>381</v>
-      </c>
-      <c r="B3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="D3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>383</v>
-      </c>
-      <c r="B4" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4">
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
         <v>5</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>14</v>
-      </c>
-      <c r="K5">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised Building and Main Find Fns
Buildings take in individual room input.
Find functions distribute adults more evenly and have been tested.
</commit_message>
<xml_diff>
--- a/documentation/TN7_Test.xlsx
+++ b/documentation/TN7_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="398">
   <si>
     <t>Church</t>
   </si>
@@ -1173,6 +1173,12 @@
     <t>Female</t>
   </si>
   <si>
+    <t>Unassigned</t>
+  </si>
+  <si>
+    <t>Sutton</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -1207,6 +1213,9 @@
   </si>
   <si>
     <t>Room Type 3 Quantity</t>
+  </si>
+  <si>
+    <t>University Baptist</t>
   </si>
 </sst>
 </file>
@@ -1289,8 +1298,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1330,7 +1345,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1338,6 +1353,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1345,6 +1363,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1758,13 +1779,13 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D2" s="2">
         <v>61704</v>
@@ -1800,13 +1821,13 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="D3" s="2">
         <v>61820</v>
@@ -2982,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3003,28 +3024,28 @@
         <v>378</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3139,6 +3160,64 @@
       </c>
       <c r="I10">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>397</v>
+      </c>
+      <c r="B11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>384</v>
+      </c>
+      <c r="B14" t="s">
+        <v>383</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>